<commit_message>
Change year to 2021
</commit_message>
<xml_diff>
--- a/media/LSR Frais Inscription.xlsx
+++ b/media/LSR Frais Inscription.xlsx
@@ -3,10 +3,10 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3602A1-094A-4A78-B73E-3F5E266304FC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62AEFFF-C32C-4D42-9831-C960C2AB0418}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="0mMFGNhDyLpF0eVlornqGqWIEY+Keivj1d5zdKC6kueANGthnCptPKZlB4TGb2Kuh9Y7C3sIbzvROXQDbVyReQ==" workbookSaltValue="0ziaGb5q8uxudE1Zb0X8jQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="20892" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="20880" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulateur" sheetId="2" r:id="rId1"/>
@@ -102,9 +102,6 @@
     <t>Nombre d'enfant (s) à charge</t>
   </si>
   <si>
-    <t>Coût total année scolaire 2020/2021</t>
-  </si>
-  <si>
     <t>Frais d'inscription (uniquement la 1ère année)</t>
   </si>
   <si>
@@ -112,10 +109,6 @@
   </si>
   <si>
     <t>Simulateur de coûts d'écolage</t>
-  </si>
-  <si>
-    <t>version 1
-15 avril 2020</t>
   </si>
   <si>
     <t>Réf. décision taxation</t>
@@ -137,6 +130,13 @@
   </si>
   <si>
     <t>3.510+530</t>
+  </si>
+  <si>
+    <t>Coût total année scolaire 2021/2022</t>
+  </si>
+  <si>
+    <t>version 1.2
+20 juin 2020</t>
   </si>
 </sst>
 </file>
@@ -637,6 +637,65 @@
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="2" applyAlignment="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="17" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0" hidden="1"/>
@@ -658,65 +717,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0" hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="2" applyAlignment="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="17" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
       <protection hidden="1"/>
@@ -728,16 +728,6 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="5">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -800,6 +790,16 @@
         <sz val="11"/>
         <color auto="1"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -870,14 +870,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2082031A-BF05-4D35-91F6-16CCCB718446}" name="Fratrie" displayName="Fratrie" ref="G2:H7" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2082031A-BF05-4D35-91F6-16CCCB718446}" name="Fratrie" displayName="Fratrie" ref="G2:H7" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="G2:H7" xr:uid="{C7B99F59-98AA-4B27-BEAC-0357A031CDA4}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G3:H7">
     <sortCondition ref="G2:G7"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{1A063431-115F-46CA-B56A-1A80709150E8}" name="Enfants" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{9B9A6617-13E2-45F2-8CA9-DDDE1128F060}" name="Rabais" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{1A063431-115F-46CA-B56A-1A80709150E8}" name="Enfants" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{9B9A6617-13E2-45F2-8CA9-DDDE1128F060}" name="Rabais" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1104,16 +1104,16 @@
   <sheetData>
     <row r="1" spans="2:6" s="28" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="52" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="49"/>
+      <c r="B2" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="64"/>
+      <c r="D2" s="65"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="2:6" ht="14.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
       <c r="E3"/>
     </row>
     <row r="4" spans="2:6" s="28" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1124,35 +1124,35 @@
         <v>14</v>
       </c>
       <c r="C5" s="68" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="68"/>
+      <c r="E5" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="68"/>
-      <c r="E5" s="56" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="57" t="s">
+      <c r="F5" s="59" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:6" s="28" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="58"/>
-      <c r="C6" s="59" t="s">
+      <c r="B6" s="56"/>
+      <c r="C6" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="59" t="s">
+      <c r="D6" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="60"/>
-      <c r="F6" s="61"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="60"/>
     </row>
     <row r="7" spans="2:6" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="64">
+      <c r="C7" s="51">
         <v>650</v>
       </c>
-      <c r="D7" s="65" t="s">
+      <c r="D7" s="52" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="29"/>
@@ -1165,10 +1165,10 @@
       <c r="B8" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="64">
+      <c r="C8" s="51">
         <v>310</v>
       </c>
-      <c r="D8" s="65" t="s">
+      <c r="D8" s="52" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="13"/>
@@ -1181,19 +1181,19 @@
       <c r="B9" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="53"/>
-      <c r="D9" s="53"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
       <c r="F9" s="9"/>
     </row>
     <row r="10" spans="2:6" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="64">
+      <c r="C10" s="51">
         <v>410</v>
       </c>
-      <c r="D10" s="67" t="s">
-        <v>35</v>
+      <c r="D10" s="54" t="s">
+        <v>33</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="9">
@@ -1203,12 +1203,12 @@
     </row>
     <row r="11" spans="2:6" s="28" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="64">
+        <v>31</v>
+      </c>
+      <c r="C11" s="51">
         <v>420</v>
       </c>
-      <c r="D11" s="66">
+      <c r="D11" s="53">
         <v>3230</v>
       </c>
       <c r="E11" s="13"/>
@@ -1219,13 +1219,13 @@
     </row>
     <row r="12" spans="2:6" s="28" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="51">
+        <v>430</v>
+      </c>
+      <c r="D12" s="53" t="s">
         <v>34</v>
-      </c>
-      <c r="C12" s="64">
-        <v>430</v>
-      </c>
-      <c r="D12" s="66" t="s">
-        <v>36</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="9">
@@ -1237,18 +1237,18 @@
       <c r="B13" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
       <c r="F13" s="9"/>
     </row>
     <row r="14" spans="2:6" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="64">
+        <v>26</v>
+      </c>
+      <c r="C14" s="51">
         <v>610</v>
       </c>
-      <c r="D14" s="65" t="s">
+      <c r="D14" s="52" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="29"/>
@@ -1261,10 +1261,10 @@
       <c r="B15" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="64">
+      <c r="C15" s="51">
         <v>540</v>
       </c>
-      <c r="D15" s="65" t="s">
+      <c r="D15" s="52" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="29"/>
@@ -1294,17 +1294,17 @@
       <c r="B18" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="63"/>
-      <c r="D18" s="63"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="50"/>
       <c r="E18" s="18"/>
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="2:6" s="28" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="62"/>
-      <c r="D19" s="62"/>
+        <v>29</v>
+      </c>
+      <c r="C19" s="61"/>
+      <c r="D19" s="61"/>
       <c r="E19" s="31"/>
       <c r="F19" s="4">
         <f>IF(OR(C19=Feuil2!E1,C19=0),0,-15600)</f>
@@ -1315,8 +1315,8 @@
       <c r="B20" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="46"/>
-      <c r="D20" s="47"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="63"/>
       <c r="E20" s="19">
         <v>-14000</v>
       </c>
@@ -1360,8 +1360,8 @@
       <c r="B24" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="50"/>
-      <c r="D24" s="51"/>
+      <c r="C24" s="66"/>
+      <c r="D24" s="67"/>
       <c r="E24" s="31"/>
       <c r="F24" s="32"/>
     </row>
@@ -1382,7 +1382,7 @@
     </row>
     <row r="26" spans="2:6" s="28" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
@@ -1408,7 +1408,7 @@
     </row>
     <row r="28" spans="2:6" ht="16.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="38" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
@@ -1429,8 +1429,8 @@
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B31" s="54" t="s">
-        <v>29</v>
+      <c r="B31" s="48" t="s">
+        <v>36</v>
       </c>
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
@@ -6307,19 +6307,19 @@
       <c r="E1005" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="ACXgOTrYN4UKXo0pVOMgXLDcUzX7lInCVSBpNwOoey5oJf5MVuU7SCMfqNWnBJCDVBHdwXLaZcXhGrIx/vwrmA==" saltValue="owRfHdaiNaNSEI62Fuy2RQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="OPiXZ1s718cagAabu4dwpWlAzI/aHbSsjgz6rsaPQAqdoE5w84izZ0qvXVBkbRT3wDk7m8vlUJRPdf7zl2E+FQ==" saltValue="YXEjopoIalKjGMTIQjKRuQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="8">
+    <mergeCell ref="C2:D3"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C5:D5"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C2:D3"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <conditionalFormatting sqref="C24:D24">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
       <formula>$C$20</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>